<commit_message>
v1.2 Fix some problems and add some new features
</commit_message>
<xml_diff>
--- a/results/Algorithm 2/results_search_encoded.xlsx
+++ b/results/Algorithm 2/results_search_encoded.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\desk_others\contribute\AE unknown number separation SPL\Supplemental Materials\code\results\Algorithm 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\desk_others\contribute\AE unknown number separation SPL\Supplemental Materials\code_results\results\Algorithm 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D34823A-E4E1-4021-9B6E-BE3649B44812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A453B7F-1752-48CB-BD05-AB6A109BCBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="21960" windowHeight="13056" xr2:uid="{B3211CC7-A965-4961-BE1A-76E847C96973}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3211CC7-A965-4961-BE1A-76E847C96973}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="32">
   <si>
     <t>MSE</t>
   </si>
@@ -100,10 +100,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>model_15_2_6_lr1e-3_ep200_RTX3090_20230406</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>lr1e-5_ep200, lr1e-4_ep200, lr1e-3_ep200, lr1e-2_ep200, lr1e-1_ep200, lr1e0_ep200, lr1e+1_ep200, lr1e+2_ep200, lr1e+3_ep200</t>
   </si>
   <si>
@@ -118,7 +114,25 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>model_15_2_6_lr1e-3_ep200_tanh_20230719</t>
+    <t>model_15_2_6_lr1e-3_ep200_tanh_gln_20230719</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>model_15_2_6_lr1e-3_ep200_tanh_cln_20230806</t>
+  </si>
+  <si>
+    <t>model_15_2_6_lr1e-3_ep200_tanh_noNL_20230805</t>
+  </si>
+  <si>
+    <t>model_15_2_6_lr1e-3_ep200_linear_gln_RTX3090_20230406</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lr1e-3_ep200, lr1e-2_ep200, lr1e-1_ep200, lr1e0_ep200</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> lr1e-3_ep200, lr1e-2_ep200, lr1e-1_ep200, lr1e0_ep200,</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -553,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E766E7-25BF-4DC3-8B53-27B0AF24AE7A}">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -576,11 +590,16 @@
     <col min="18" max="18" width="9.5546875" customWidth="1"/>
     <col min="20" max="20" width="11.6640625" customWidth="1"/>
     <col min="21" max="21" width="8.109375" customWidth="1"/>
-    <col min="22" max="22" width="10" style="2" customWidth="1"/>
-    <col min="23" max="23" width="8.33203125" customWidth="1"/>
+    <col min="22" max="22" width="9.109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="9.5546875" customWidth="1"/>
+    <col min="25" max="25" width="11.6640625" customWidth="1"/>
+    <col min="26" max="26" width="8.109375" customWidth="1"/>
+    <col min="27" max="27" width="10" style="2" customWidth="1"/>
+    <col min="28" max="28" width="8.33203125" customWidth="1"/>
+    <col min="30" max="30" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -638,8 +657,32 @@
       <c r="W1" t="s">
         <v>3</v>
       </c>
+      <c r="Y1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -680,17 +723,37 @@
       </c>
       <c r="R2" s="7"/>
       <c r="T2" s="4">
+        <v>6.6279093734919999E-3</v>
+      </c>
+      <c r="U2" s="7">
+        <v>0.19125479459762501</v>
+      </c>
+      <c r="V2" s="7">
+        <v>-19.382184982299801</v>
+      </c>
+      <c r="W2" s="7"/>
+      <c r="Y2" s="4">
+        <v>7.9705705866217596E-3</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>0.19025675952434501</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>-16.195070266723601</v>
+      </c>
+      <c r="AB2" s="7"/>
+      <c r="AD2" s="4">
         <v>4.3731490150093998E-3</v>
       </c>
-      <c r="U2" s="7">
+      <c r="AE2" s="7">
         <v>0.51531398296356201</v>
       </c>
-      <c r="V2" s="7">
+      <c r="AF2" s="7">
         <v>-8.3419828414916992</v>
       </c>
-      <c r="W2" s="7"/>
+      <c r="AG2" s="7"/>
     </row>
-    <row r="3" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -731,17 +794,37 @@
       </c>
       <c r="R3" s="6"/>
       <c r="T3" s="3">
+        <v>4.5174532569944798E-3</v>
+      </c>
+      <c r="U3" s="6">
+        <v>0.76635086536407404</v>
+      </c>
+      <c r="V3" s="6">
+        <v>1.7351480722427299</v>
+      </c>
+      <c r="W3" s="6"/>
+      <c r="Y3" s="3">
+        <v>1.02889146655797E-2</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>0.65440350770950295</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>-0.55259740352630604</v>
+      </c>
+      <c r="AB3" s="6"/>
+      <c r="AD3" s="3">
         <v>8.8940616697072896E-3</v>
       </c>
-      <c r="U3" s="6">
+      <c r="AE3" s="6">
         <v>0.79667043685912997</v>
       </c>
-      <c r="V3" s="6">
+      <c r="AF3" s="6">
         <v>2.5516591072082502</v>
       </c>
-      <c r="W3" s="6"/>
+      <c r="AG3" s="6"/>
     </row>
-    <row r="4" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -782,17 +865,37 @@
       </c>
       <c r="R4" s="7"/>
       <c r="T4" s="4">
+        <v>1.3626945205032799E-2</v>
+      </c>
+      <c r="U4" s="7">
+        <v>0.18605783581733701</v>
+      </c>
+      <c r="V4" s="7">
+        <v>-16.3257732391357</v>
+      </c>
+      <c r="W4" s="7"/>
+      <c r="Y4" s="4">
+        <v>9.4622597098350508E-3</v>
+      </c>
+      <c r="Z4" s="7">
+        <v>0.49867004156112599</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>-5.4333806037902797</v>
+      </c>
+      <c r="AB4" s="7"/>
+      <c r="AD4" s="4">
         <v>1.1652720160782301E-2</v>
       </c>
-      <c r="U4" s="7">
+      <c r="AE4" s="7">
         <v>0.76348799467086703</v>
       </c>
-      <c r="V4" s="7">
+      <c r="AF4" s="7">
         <v>1.69174969196319</v>
       </c>
-      <c r="W4" s="7"/>
+      <c r="AG4" s="7"/>
     </row>
-    <row r="5" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -833,17 +936,37 @@
       </c>
       <c r="R5" s="6"/>
       <c r="T5" s="3">
+        <v>7.8445961698889698E-3</v>
+      </c>
+      <c r="U5" s="6">
+        <v>0.56098979711532504</v>
+      </c>
+      <c r="V5" s="6">
+        <v>-4.2439541816711399</v>
+      </c>
+      <c r="W5" s="6"/>
+      <c r="Y5" s="3">
+        <v>7.0875729434192103E-3</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>0.70861315727233798</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>0.34793630242347701</v>
+      </c>
+      <c r="AB5" s="6"/>
+      <c r="AD5" s="3">
         <v>5.7661617174744597E-3</v>
       </c>
-      <c r="U5" s="6">
+      <c r="AE5" s="6">
         <v>0.91062045097350997</v>
       </c>
-      <c r="V5" s="6">
+      <c r="AF5" s="6">
         <v>7.2667922973632804</v>
       </c>
-      <c r="W5" s="6"/>
+      <c r="AG5" s="6"/>
     </row>
-    <row r="6" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -890,19 +1013,43 @@
         <v>-2.9929934069514198E-2</v>
       </c>
       <c r="T6" s="4">
+        <v>1.0581768117844999E-2</v>
+      </c>
+      <c r="U6" s="7">
+        <v>0.55651146173477095</v>
+      </c>
+      <c r="V6" s="7">
+        <v>-3.52638435363769</v>
+      </c>
+      <c r="W6" s="7">
+        <v>-0.22573868930339799</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>9.0816123411059293E-3</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>0.56794434785842896</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>-3.4190425872802699</v>
+      </c>
+      <c r="AB6" s="7">
+        <v>1.12449491024017</v>
+      </c>
+      <c r="AD6" s="4">
         <v>9.1924127191305108E-3</v>
       </c>
-      <c r="U6" s="7">
+      <c r="AE6" s="7">
         <v>0.57800734043121305</v>
       </c>
-      <c r="V6" s="7">
+      <c r="AF6" s="7">
         <v>-3.0064313411712602</v>
       </c>
-      <c r="W6" s="7">
+      <c r="AG6" s="7">
         <v>1.3084819316864</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -949,19 +1096,43 @@
         <v>-0.42196533083915699</v>
       </c>
       <c r="T7" s="3">
+        <v>1.31369102746248E-2</v>
+      </c>
+      <c r="U7" s="6">
+        <v>0.18858595192432401</v>
+      </c>
+      <c r="V7" s="6">
+        <v>-16.014629364013601</v>
+      </c>
+      <c r="W7" s="6">
+        <v>-0.38854122161865201</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>1.14922998473048E-2</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>0.402686446905136</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>-7.8195333480834899</v>
+      </c>
+      <c r="AB7" s="6">
+        <v>-0.90400910377502397</v>
+      </c>
+      <c r="AD7" s="3">
         <v>1.0801991447806299E-2</v>
       </c>
-      <c r="U7" s="6">
+      <c r="AE7" s="6">
         <v>0.56709307432174605</v>
       </c>
-      <c r="V7" s="6">
+      <c r="AF7" s="6">
         <v>-3.2799546718597399</v>
       </c>
-      <c r="W7" s="6">
+      <c r="AG7" s="6">
         <v>0.96250742673873901</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1008,19 +1179,43 @@
         <v>-1.3605237938463599E-2</v>
       </c>
       <c r="T8" s="4">
+        <v>1.0954800993204099E-2</v>
+      </c>
+      <c r="U8" s="7">
+        <v>0.55365425348281805</v>
+      </c>
+      <c r="V8" s="7">
+        <v>-3.58824110031127</v>
+      </c>
+      <c r="W8" s="7">
+        <v>-0.16853305697441101</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>9.4349281862378103E-3</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>0.58169603347778298</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>-3.0490489006042401</v>
+      </c>
+      <c r="AB8" s="7">
+        <v>1.17811620235443</v>
+      </c>
+      <c r="AD8" s="4">
         <v>8.9304773136973294E-3</v>
       </c>
-      <c r="U8" s="7">
+      <c r="AE8" s="7">
         <v>0.59111291170120195</v>
       </c>
-      <c r="V8" s="7">
+      <c r="AF8" s="7">
         <v>-2.68426012992858</v>
       </c>
-      <c r="W8" s="7">
+      <c r="AG8" s="7">
         <v>1.5707479715347199</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1067,19 +1262,43 @@
         <v>-0.37161320447921697</v>
       </c>
       <c r="T9" s="3">
+        <v>9.9577363580465299E-3</v>
+      </c>
+      <c r="U9" s="6">
+        <v>0.46141937375068598</v>
+      </c>
+      <c r="V9" s="6">
+        <v>-6.4508309364318803</v>
+      </c>
+      <c r="W9" s="6">
+        <v>0.72873884439468295</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>9.3271639198064804E-3</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>0.54348725080490101</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>-3.95782017707824</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>0.99668842554092396</v>
+      </c>
+      <c r="AD9" s="3">
         <v>7.7286479063332003E-3</v>
       </c>
-      <c r="U9" s="6">
+      <c r="AE9" s="6">
         <v>0.66784864664077703</v>
       </c>
-      <c r="V9" s="6">
+      <c r="AF9" s="6">
         <v>-0.81013238430023105</v>
       </c>
-      <c r="W9" s="6">
+      <c r="AG9" s="6">
         <v>2.3812701702117902</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1126,19 +1345,43 @@
         <v>-0.50237047672271695</v>
       </c>
       <c r="T10" s="4">
+        <v>1.3502164743840601E-2</v>
+      </c>
+      <c r="U10" s="7">
+        <v>0.18556512892246199</v>
+      </c>
+      <c r="V10" s="7">
+        <v>-15.796422958374</v>
+      </c>
+      <c r="W10" s="7">
+        <v>-0.392739027738571</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>1.19071248918771E-2</v>
+      </c>
+      <c r="Z10" s="7">
+        <v>0.41181135177612299</v>
+      </c>
+      <c r="AA10" s="7">
+        <v>-7.5406408309936497</v>
+      </c>
+      <c r="AB10" s="7">
+        <v>-0.80354279279708796</v>
+      </c>
+      <c r="AD10" s="4">
         <v>1.0008207522332601E-2</v>
       </c>
-      <c r="U10" s="7">
+      <c r="AE10" s="7">
         <v>0.59352701902389504</v>
       </c>
-      <c r="V10" s="7">
+      <c r="AF10" s="7">
         <v>-2.6313924789428702</v>
       </c>
-      <c r="W10" s="7">
+      <c r="AG10" s="7">
         <v>1.2356650829315099</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1185,19 +1428,43 @@
         <v>-0.40590006113052302</v>
       </c>
       <c r="T11" s="4">
+        <v>1.0447448119521099E-2</v>
+      </c>
+      <c r="U11" s="7">
+        <v>0.462138712406158</v>
+      </c>
+      <c r="V11" s="7">
+        <v>-6.4842905998229901</v>
+      </c>
+      <c r="W11" s="7">
+        <v>0.52727216482162398</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>9.51414089649915E-3</v>
+      </c>
+      <c r="Z11" s="7">
+        <v>0.54438340663909901</v>
+      </c>
+      <c r="AA11" s="7">
+        <v>-3.9503035545349099</v>
+      </c>
+      <c r="AB11" s="7">
+        <v>0.90874212980270297</v>
+      </c>
+      <c r="AD11" s="4">
         <v>7.74739729240536E-3</v>
       </c>
-      <c r="U11" s="7">
+      <c r="AE11" s="7">
         <v>0.66633862257003695</v>
       </c>
-      <c r="V11" s="7">
+      <c r="AF11" s="7">
         <v>-0.75322437286376898</v>
       </c>
-      <c r="W11" s="7">
+      <c r="AG11" s="7">
         <v>2.32456302642822</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1244,19 +1511,43 @@
         <v>-1.3702493160962999E-2</v>
       </c>
       <c r="T12" s="4">
+        <v>1.6085289418697302E-2</v>
+      </c>
+      <c r="U12" s="7">
+        <v>0.455864667892456</v>
+      </c>
+      <c r="V12" s="7">
+        <v>-5.9200930595397896</v>
+      </c>
+      <c r="W12" s="7">
+        <v>-1.7828993797302199</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>1.00644901394844E-2</v>
+      </c>
+      <c r="Z12" s="7">
+        <v>0.48172909021377502</v>
+      </c>
+      <c r="AA12" s="7">
+        <v>-5.4549403190612704</v>
+      </c>
+      <c r="AB12" s="7">
+        <v>0.943883717060089</v>
+      </c>
+      <c r="AD12" s="4">
         <v>9.9526401609182306E-3</v>
       </c>
-      <c r="U12" s="7">
+      <c r="AE12" s="7">
         <v>0.48409858345985401</v>
       </c>
-      <c r="V12" s="7">
+      <c r="AF12" s="7">
         <v>-5.2294559478759703</v>
       </c>
-      <c r="W12" s="7">
+      <c r="AG12" s="7">
         <v>1.0717428922653101</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1303,19 +1594,43 @@
         <v>-2.3388376235961901</v>
       </c>
       <c r="T13" s="4">
+        <v>1.3442295603454101E-2</v>
+      </c>
+      <c r="U13" s="7">
+        <v>0.189014837145805</v>
+      </c>
+      <c r="V13" s="7">
+        <v>-15.7342777252197</v>
+      </c>
+      <c r="W13" s="7">
+        <v>-0.35020223259925798</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>1.43403001129627E-2</v>
+      </c>
+      <c r="Z13" s="7">
+        <v>0.35849374532699502</v>
+      </c>
+      <c r="AA13" s="7">
+        <v>-8.8944387435912997</v>
+      </c>
+      <c r="AB13" s="7">
+        <v>-1.56288802623748</v>
+      </c>
+      <c r="AD13" s="4">
         <v>1.0463281534612101E-2</v>
       </c>
-      <c r="U13" s="7">
+      <c r="AE13" s="7">
         <v>0.498912513256073</v>
       </c>
-      <c r="V13" s="7">
+      <c r="AF13" s="7">
         <v>-4.9540491104125897</v>
       </c>
-      <c r="W13" s="7">
+      <c r="AG13" s="7">
         <v>1.00149774551391</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1362,19 +1677,47 @@
         <v>-0.50394803285598699</v>
       </c>
       <c r="T14" s="4">
+        <v>1.25766228884458E-2</v>
+      </c>
+      <c r="U14" s="7">
+        <v>0.40258273482322599</v>
+      </c>
+      <c r="V14" s="7">
+        <v>-7.7898459434509197</v>
+      </c>
+      <c r="W14" s="7">
+        <v>-0.19812816381454401</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>1.10710151493549E-2</v>
+      </c>
+      <c r="Z14" s="7">
+        <v>0.45635741949081399</v>
+      </c>
+      <c r="AA14" s="7">
+        <v>-6.0918879508972097</v>
+      </c>
+      <c r="AB14" s="7">
+        <v>0.23240281641483301</v>
+      </c>
+      <c r="AD14" s="4">
         <v>9.5588220283389091E-3</v>
       </c>
-      <c r="U14" s="7">
+      <c r="AE14" s="7">
         <v>0.55508649349212602</v>
       </c>
-      <c r="V14" s="7">
+      <c r="AF14" s="7">
         <v>-3.5603487491607599</v>
       </c>
-      <c r="W14" s="7">
+      <c r="AG14" s="7">
         <v>1.38361740112304</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AD15" s="2"/>
+      <c r="AF15" s="2"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>15</v>
       </c>
@@ -1417,18 +1760,42 @@
       </c>
       <c r="T16" s="2">
         <f>AVERAGE(T2:T5)</f>
-        <v>7.6715231407433627E-3</v>
+        <v>8.1542260013520614E-3</v>
       </c>
       <c r="U16" s="8">
         <f t="shared" ref="U16:V16" si="3">AVERAGE(U2:U5)</f>
-        <v>0.74652321636676722</v>
+        <v>0.4261633232235903</v>
       </c>
       <c r="V16" s="1">
         <f t="shared" si="3"/>
+        <v>-9.5541910827159775</v>
+      </c>
+      <c r="Y16" s="2">
+        <f>AVERAGE(Y2:Y5)</f>
+        <v>8.7023294763639309E-3</v>
+      </c>
+      <c r="Z16" s="8">
+        <f t="shared" ref="Z16:AA16" si="4">AVERAGE(Z2:Z5)</f>
+        <v>0.51298586651682798</v>
+      </c>
+      <c r="AA16" s="1">
+        <f t="shared" si="4"/>
+        <v>-5.4582779929041774</v>
+      </c>
+      <c r="AD16" s="2">
+        <f>AVERAGE(AD2:AD5)</f>
+        <v>7.6715231407433627E-3</v>
+      </c>
+      <c r="AE16" s="8">
+        <f t="shared" ref="AE16:AF16" si="5">AVERAGE(AE2:AE5)</f>
+        <v>0.74652321636676722</v>
+      </c>
+      <c r="AF16" s="1">
+        <f t="shared" si="5"/>
         <v>0.79205456376075545</v>
       </c>
     </row>
-    <row r="17" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>16</v>
       </c>
@@ -1437,15 +1804,15 @@
         <v>8.4924451075494255E-3</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" ref="F17:H17" si="4">AVERAGE(F6:F11)</f>
+        <f t="shared" ref="F17:H17" si="6">AVERAGE(F6:F11)</f>
         <v>0.67620866497357623</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.53625870247681873</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9391189614931683</v>
       </c>
       <c r="J17" s="2">
@@ -1453,15 +1820,15 @@
         <v>1.1968845191101184E-2</v>
       </c>
       <c r="K17" s="8">
-        <f t="shared" ref="K17:M17" si="5">AVERAGE(K6:K11)</f>
+        <f t="shared" ref="K17:M17" si="7">AVERAGE(K6:K11)</f>
         <v>0.35908580323060318</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-9.2302789688110192</v>
       </c>
       <c r="M17" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.61152226908597862</v>
       </c>
       <c r="O17" s="2">
@@ -1469,35 +1836,67 @@
         <v>1.1951142145941616E-2</v>
       </c>
       <c r="P17" s="8">
-        <f t="shared" ref="P17:R17" si="6">AVERAGE(P6:P11)</f>
+        <f t="shared" ref="P17:R17" si="8">AVERAGE(P6:P11)</f>
         <v>0.33649219324191365</v>
       </c>
       <c r="Q17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-12.692541837692238</v>
       </c>
       <c r="R17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-0.29089737419659861</v>
       </c>
       <c r="T17" s="2">
         <f>AVERAGE(T6:T11)</f>
+        <v>1.1430138101180355E-2</v>
+      </c>
+      <c r="U17" s="8">
+        <f t="shared" ref="U17:W17" si="9">AVERAGE(U6:U11)</f>
+        <v>0.40131248037020323</v>
+      </c>
+      <c r="V17" s="1">
+        <f t="shared" si="9"/>
+        <v>-8.6434665520985714</v>
+      </c>
+      <c r="W17" s="1">
+        <f t="shared" si="9"/>
+        <v>1.3409835596879147E-2</v>
+      </c>
+      <c r="Y17" s="2">
+        <f>AVERAGE(Y6:Y11)</f>
+        <v>1.0126211680471878E-2</v>
+      </c>
+      <c r="Z17" s="8">
+        <f t="shared" ref="Z17:AB17" si="10">AVERAGE(Z6:Z11)</f>
+        <v>0.50866813957691182</v>
+      </c>
+      <c r="AA17" s="1">
+        <f t="shared" si="10"/>
+        <v>-4.9560648997624659</v>
+      </c>
+      <c r="AB17" s="1">
+        <f t="shared" si="10"/>
+        <v>0.41674829522768581</v>
+      </c>
+      <c r="AD17" s="2">
+        <f>AVERAGE(AD6:AD11)</f>
         <v>9.0681890336175505E-3</v>
       </c>
-      <c r="U17" s="8">
-        <f t="shared" ref="U17:W17" si="7">AVERAGE(U6:U11)</f>
+      <c r="AE17" s="8">
+        <f t="shared" ref="AE17:AG17" si="11">AVERAGE(AE6:AE11)</f>
         <v>0.61065460244814496</v>
       </c>
-      <c r="V17" s="1">
-        <f t="shared" si="7"/>
+      <c r="AF17" s="1">
+        <f t="shared" si="11"/>
         <v>-2.1942325631777422</v>
       </c>
-      <c r="W17" s="1">
-        <f t="shared" si="7"/>
+      <c r="AG17" s="1">
+        <f t="shared" si="11"/>
         <v>1.6305392682552295</v>
       </c>
     </row>
-    <row r="18" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>17</v>
       </c>
@@ -1506,15 +1905,15 @@
         <v>9.5731609811385444E-3</v>
       </c>
       <c r="F18" s="8">
-        <f t="shared" ref="F18:H18" si="8">AVERAGE(F12:F14)</f>
+        <f t="shared" ref="F18:H18" si="12">AVERAGE(F12:F14)</f>
         <v>0.55437904596328702</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>-3.5609539349873831</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1.4095589717229167</v>
       </c>
       <c r="J18" s="2">
@@ -1522,15 +1921,15 @@
         <v>1.3093251114090232E-2</v>
       </c>
       <c r="K18" s="8">
-        <f t="shared" ref="K18:M18" si="9">AVERAGE(K12:K14)</f>
+        <f t="shared" ref="K18:M18" si="13">AVERAGE(K12:K14)</f>
         <v>0.32633536060651097</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-9.9655046463012482</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-0.89651879668235557</v>
       </c>
       <c r="O18" s="2">
@@ -1538,35 +1937,67 @@
         <v>1.4347489612797831E-2</v>
       </c>
       <c r="P18" s="8">
-        <f t="shared" ref="P18:R18" si="10">AVERAGE(P12:P14)</f>
+        <f t="shared" ref="P18:R18" si="14">AVERAGE(P12:P14)</f>
         <v>0.30060291290283164</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-13.235350290934198</v>
       </c>
       <c r="R18" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-0.95216271653771345</v>
       </c>
       <c r="T18" s="2">
         <f>AVERAGE(T12:T14)</f>
+        <v>1.4034735970199066E-2</v>
+      </c>
+      <c r="U18" s="8">
+        <f t="shared" ref="U18:W18" si="15">AVERAGE(U12:U14)</f>
+        <v>0.34915407995382902</v>
+      </c>
+      <c r="V18" s="1">
+        <f t="shared" si="15"/>
+        <v>-9.81473890940347</v>
+      </c>
+      <c r="W18" s="1">
+        <f t="shared" si="15"/>
+        <v>-0.77707659204800716</v>
+      </c>
+      <c r="Y18" s="2">
+        <f>AVERAGE(Y12:Y14)</f>
+        <v>1.1825268467267334E-2</v>
+      </c>
+      <c r="Z18" s="8">
+        <f t="shared" ref="Z18:AB18" si="16">AVERAGE(Z12:Z14)</f>
+        <v>0.43219341834386132</v>
+      </c>
+      <c r="AA18" s="1">
+        <f t="shared" si="16"/>
+        <v>-6.8137556711832596</v>
+      </c>
+      <c r="AB18" s="1">
+        <f t="shared" si="16"/>
+        <v>-0.12886716425418601</v>
+      </c>
+      <c r="AD18" s="2">
+        <f>AVERAGE(AD12:AD14)</f>
         <v>9.9915812412897462E-3</v>
       </c>
-      <c r="U18" s="8">
-        <f t="shared" ref="U18:W18" si="11">AVERAGE(U12:U14)</f>
+      <c r="AE18" s="8">
+        <f t="shared" ref="AE18:AG18" si="17">AVERAGE(AE12:AE14)</f>
         <v>0.51269919673601771</v>
       </c>
-      <c r="V18" s="1">
-        <f t="shared" si="11"/>
+      <c r="AF18" s="1">
+        <f t="shared" si="17"/>
         <v>-4.5812846024831062</v>
       </c>
-      <c r="W18" s="1">
-        <f t="shared" si="11"/>
+      <c r="AG18" s="1">
+        <f t="shared" si="17"/>
         <v>1.1522860129674199</v>
       </c>
     </row>
-    <row r="19" spans="3:23" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:33" ht="15.6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>18</v>
       </c>
@@ -1575,19 +2006,26 @@
       </c>
       <c r="G19"/>
       <c r="J19" s="5" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="L19"/>
       <c r="O19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q19"/>
       <c r="T19" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="V19"/>
+      <c r="Y19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA19"/>
+      <c r="AD19" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="20" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:33" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>19</v>
       </c>
@@ -1595,14 +2033,21 @@
         <v>21</v>
       </c>
       <c r="J20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" t="s">
+        <v>25</v>
+      </c>
+      <c r="T20" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD20" t="s">
         <v>23</v>
       </c>
-      <c r="O20" t="s">
-        <v>26</v>
-      </c>
-      <c r="T20" t="s">
-        <v>24</v>
-      </c>
+      <c r="AF20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>